<commit_message>
refactor and update excel
</commit_message>
<xml_diff>
--- a/ReactjswithF8.xlsx
+++ b/ReactjswithF8.xlsx
@@ -1,41 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cng\0_personal\2_Reactjs\1_Reactjs_with_F8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cng\study\reactjs\reactjs_f8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED63A1C0-3651-4F3E-BDD9-72E1005CB80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBE756C-1455-4CF1-89EA-DB263C2CB856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2505" windowWidth="24698" windowHeight="11535" xr2:uid="{4149283A-B59B-4AE5-95CD-24380AF48A33}"/>
+    <workbookView xWindow="58695" yWindow="750" windowWidth="25530" windowHeight="11265" xr2:uid="{4149283A-B59B-4AE5-95CD-24380AF48A33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="note" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Rest trong js là gì?</t>
   </si>
@@ -54,16 +45,36 @@
   <si>
     <t>Destructurning : phân rã các giá trị</t>
   </si>
+  <si>
+    <t>Reactjs: nhungs unpack link (CDN) vào dự án.</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>&lt;script src="https://unpkg.com/react@17/umd/react.development.js" crossorigin&gt;&lt;/script&gt;</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Sử dụng DOM và React để hiển thị nội dung trong html.</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Hien thị list ul-li với react</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="3"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -71,7 +82,7 @@
     <font>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -80,8 +91,15 @@
       <b/>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -118,7 +136,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -188,9 +206,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>320754</xdr:colOff>
+      <xdr:colOff>325516</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>164521</xdr:rowOff>
+      <xdr:rowOff>169283</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -302,9 +320,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>470630</xdr:colOff>
+      <xdr:colOff>475392</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>158099</xdr:rowOff>
+      <xdr:rowOff>162861</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -558,7 +576,7 @@
       <xdr:col>35</xdr:col>
       <xdr:colOff>153102</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>196775</xdr:rowOff>
+      <xdr:rowOff>201537</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -754,7 +772,7 @@
       <xdr:col>33</xdr:col>
       <xdr:colOff>573158</xdr:colOff>
       <xdr:row>85</xdr:row>
-      <xdr:rowOff>90461</xdr:rowOff>
+      <xdr:rowOff>95223</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -796,7 +814,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>130382</xdr:colOff>
+      <xdr:colOff>135144</xdr:colOff>
       <xdr:row>104</xdr:row>
       <xdr:rowOff>47854</xdr:rowOff>
     </xdr:to>
@@ -840,7 +858,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>623022</xdr:colOff>
+      <xdr:colOff>627784</xdr:colOff>
       <xdr:row>124</xdr:row>
       <xdr:rowOff>106725</xdr:rowOff>
     </xdr:to>
@@ -1073,6 +1091,548 @@
             <a:t> tên như này thì sẽ không bị đè lên nhau</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="2400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>38415</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>87913</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1436A99-AD4C-480B-9803-1249D7387518}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2738438" y="59102625"/>
+          <a:ext cx="14749778" cy="6564913"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>528637</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>357185</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>692726</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>380124</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AEE5C7A-88E5-4B6B-BEA8-F92CBD852FF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17983200" y="59054998"/>
+          <a:ext cx="8448674" cy="10138489"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>51954</xdr:colOff>
+      <xdr:row>178</xdr:row>
+      <xdr:rowOff>363682</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>668058</xdr:colOff>
+      <xdr:row>192</xdr:row>
+      <xdr:rowOff>30487</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC888115-0336-4DE4-A5AA-02C5F5DE1667}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1610590" y="74346955"/>
+          <a:ext cx="10309524" cy="5480952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>103909</xdr:colOff>
+      <xdr:row>196</xdr:row>
+      <xdr:rowOff>173182</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>523562</xdr:colOff>
+      <xdr:row>205</xdr:row>
+      <xdr:rowOff>227692</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{129CAFD8-45FC-48DE-923D-9AB72339F849}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1662545" y="81637909"/>
+          <a:ext cx="16352381" cy="3790476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>74035</xdr:colOff>
+      <xdr:row>195</xdr:row>
+      <xdr:rowOff>294409</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>398318</xdr:colOff>
+      <xdr:row>199</xdr:row>
+      <xdr:rowOff>333808</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="TextBox 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6CC5E7C-A28C-489D-9EA4-20C6B10B60C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9945399" y="81343500"/>
+          <a:ext cx="6558828" cy="1701944"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B0F0"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400"/>
+            <a:t>craeteElement thì</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" baseline="0"/>
+            <a:t> phần tử thứ</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" baseline="0"/>
+            <a:t>1.là type</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" baseline="0"/>
+            <a:t>2.prop ( Thuộc tính, cái mà sẽ thêm id, style..vv)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" baseline="0"/>
+            <a:t>3.content</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>658090</xdr:colOff>
+      <xdr:row>197</xdr:row>
+      <xdr:rowOff>34636</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>585998</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>398319</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFB59BB5-0EF7-4223-86F4-43EF74B802D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18149454" y="81915000"/>
+          <a:ext cx="8240635" cy="2441864"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>173182</xdr:colOff>
+      <xdr:row>209</xdr:row>
+      <xdr:rowOff>155864</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>613615</xdr:colOff>
+      <xdr:row>223</xdr:row>
+      <xdr:rowOff>94098</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF4711F5-48C3-4C8B-B15C-6BE1C427D32D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1731818" y="87023864"/>
+          <a:ext cx="12909524" cy="5757143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>632980</xdr:colOff>
+      <xdr:row>207</xdr:row>
+      <xdr:rowOff>195262</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>264536</xdr:colOff>
+      <xdr:row>209</xdr:row>
+      <xdr:rowOff>281853</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="TextBox 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C54BA92-4AEE-459D-9CB6-0640E0AA6791}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2884344" y="86231989"/>
+          <a:ext cx="6558828" cy="917864"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B0F0"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400"/>
+            <a:t>add style</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" baseline="0"/>
+            <a:t> for react</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>780833</xdr:colOff>
+      <xdr:row>200</xdr:row>
+      <xdr:rowOff>294408</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>277091</xdr:colOff>
+      <xdr:row>213</xdr:row>
+      <xdr:rowOff>316489</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="Freeform: Shape 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98118700-59FC-41BF-B8C4-F23F58CF01F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="780833" y="83421681"/>
+          <a:ext cx="3133076" cy="5425353"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 2600974 w 3068565"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 5853546"/>
+            <a:gd name="connsiteX1" fmla="*/ 3247 w 3068565"/>
+            <a:gd name="connsiteY1" fmla="*/ 2684318 h 5853546"/>
+            <a:gd name="connsiteX2" fmla="*/ 3068565 w 3068565"/>
+            <a:gd name="connsiteY2" fmla="*/ 5853546 h 5853546"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="3068565" h="5853546">
+              <a:moveTo>
+                <a:pt x="2600974" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="1263144" y="854363"/>
+                <a:pt x="-74685" y="1708727"/>
+                <a:pt x="3247" y="2684318"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="81179" y="3659909"/>
+                <a:pt x="1574872" y="4756727"/>
+                <a:pt x="3068565" y="5853546"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="stealth" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1495,19 +2055,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2983FCD5-2F3F-4DE5-AD03-9AA1FE5631D5}">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:L207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Z124" sqref="Z124"/>
+    <sheetView tabSelected="1" topLeftCell="A193" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C209" sqref="C209"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="25.5"/>
+  <sheetFormatPr defaultColWidth="9.0625" defaultRowHeight="32.25" x14ac:dyDescent="1.25"/>
   <cols>
-    <col min="1" max="1" width="20.46484375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.06640625" style="1"/>
+    <col min="1" max="1" width="20.4375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.0625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="1.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1523,12 +2083,12 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="1.25">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="1.25">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -1544,17 +2104,17 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="1.25">
       <c r="B29" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="1.25">
       <c r="D31" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="1.25">
       <c r="A49" s="2" t="s">
         <v>5</v>
       </c>
@@ -1570,7 +2130,66 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="1.25">
+      <c r="A144" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B144" s="2"/>
+      <c r="C144" s="2"/>
+      <c r="D144" s="2"/>
+      <c r="E144" s="2"/>
+      <c r="F144" s="2"/>
+      <c r="G144" s="2"/>
+      <c r="H144" s="2"/>
+      <c r="I144" s="2"/>
+      <c r="J144" s="2"/>
+      <c r="K144" s="2"/>
+      <c r="L144" s="2"/>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="1.25">
+      <c r="B145" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12" x14ac:dyDescent="1.25">
+      <c r="A178" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B178" s="2"/>
+      <c r="C178" s="2"/>
+      <c r="D178" s="2"/>
+      <c r="E178" s="2"/>
+      <c r="F178" s="2"/>
+      <c r="G178" s="2"/>
+      <c r="H178" s="2"/>
+      <c r="I178" s="2"/>
+      <c r="J178" s="2"/>
+      <c r="K178" s="2"/>
+      <c r="L178" s="2"/>
+    </row>
+    <row r="195" spans="1:12" x14ac:dyDescent="1.25">
+      <c r="A195" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B195" s="2"/>
+      <c r="C195" s="2"/>
+      <c r="D195" s="2"/>
+      <c r="E195" s="2"/>
+      <c r="F195" s="2"/>
+      <c r="G195" s="2"/>
+      <c r="H195" s="2"/>
+      <c r="I195" s="2"/>
+      <c r="J195" s="2"/>
+      <c r="K195" s="2"/>
+      <c r="L195" s="2"/>
+    </row>
+    <row r="207" spans="1:12" x14ac:dyDescent="1.25">
+      <c r="E207" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1585,8 +2204,9 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
   <sheetData/>
+  <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
add JSX - babel for react
</commit_message>
<xml_diff>
--- a/ReactjswithF8.xlsx
+++ b/ReactjswithF8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cng\study\reactjs\reactjs_f8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cng\0_personal\2_Reactjs\1_Reactjs_with_F8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBE756C-1455-4CF1-89EA-DB263C2CB856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9869AD5D-DEB9-4499-961F-9AB37D8113AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58695" yWindow="750" windowWidth="25530" windowHeight="11265" xr2:uid="{4149283A-B59B-4AE5-95CD-24380AF48A33}"/>
+    <workbookView xWindow="57165" yWindow="1530" windowWidth="21600" windowHeight="11430" xr2:uid="{4149283A-B59B-4AE5-95CD-24380AF48A33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Rest trong js là gì?</t>
   </si>
@@ -65,16 +65,25 @@
     <t xml:space="preserve"> </t>
     <phoneticPr fontId="3"/>
   </si>
+  <si>
+    <t>Sử dụng ReactDOM để hiển thị HTML text ( hiển thị lên màn hình)</t>
+  </si>
+  <si>
+    <t>React DOM -&gt; render UL LI to UI</t>
+  </si>
+  <si>
+    <t>React DOM - Render UI với @React18</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -82,7 +91,7 @@
     <font>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -91,13 +100,13 @@
       <b/>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -136,7 +145,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1148,10 +1157,10 @@
       <xdr:rowOff>357185</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>692726</xdr:colOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>9090</xdr:colOff>
       <xdr:row>170</xdr:row>
-      <xdr:rowOff>380124</xdr:rowOff>
+      <xdr:rowOff>322974</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1192,8 +1201,8 @@
       <xdr:rowOff>363682</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>668058</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>8236</xdr:colOff>
       <xdr:row>192</xdr:row>
       <xdr:rowOff>30487</xdr:rowOff>
     </xdr:to>
@@ -1276,14 +1285,14 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>74035</xdr:colOff>
-      <xdr:row>195</xdr:row>
-      <xdr:rowOff>294409</xdr:rowOff>
+      <xdr:row>192</xdr:row>
+      <xdr:rowOff>294410</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>398318</xdr:colOff>
       <xdr:row>199</xdr:row>
-      <xdr:rowOff>333808</xdr:rowOff>
+      <xdr:rowOff>324284</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1298,8 +1307,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9945399" y="81343500"/>
-          <a:ext cx="6558828" cy="1701944"/>
+          <a:off x="9235353" y="63471137"/>
+          <a:ext cx="6091238" cy="2333192"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1378,9 +1387,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
-      <xdr:colOff>585998</xdr:colOff>
+      <xdr:colOff>590760</xdr:colOff>
       <xdr:row>202</xdr:row>
-      <xdr:rowOff>398319</xdr:rowOff>
+      <xdr:rowOff>322119</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1422,7 +1431,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>613615</xdr:colOff>
+      <xdr:colOff>618377</xdr:colOff>
       <xdr:row>223</xdr:row>
       <xdr:rowOff>94098</xdr:rowOff>
     </xdr:to>
@@ -1633,6 +1642,675 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>477236</xdr:colOff>
+      <xdr:row>230</xdr:row>
+      <xdr:rowOff>91353</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>420399</xdr:colOff>
+      <xdr:row>250</xdr:row>
+      <xdr:rowOff>304516</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="図 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F01DDEC-C29E-4BB7-90C2-70DFDEF10726}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1949281" y="75771808"/>
+          <a:ext cx="9554754" cy="6789310"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>477115</xdr:colOff>
+      <xdr:row>231</xdr:row>
+      <xdr:rowOff>143308</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>102542</xdr:colOff>
+      <xdr:row>242</xdr:row>
+      <xdr:rowOff>26843</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="図 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D1B23C1-B4E7-43AB-A6BD-FBBCF38E3FF6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12842297" y="76152808"/>
+          <a:ext cx="7314700" cy="3503035"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>234</xdr:row>
+      <xdr:rowOff>34637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>242454</xdr:colOff>
+      <xdr:row>238</xdr:row>
+      <xdr:rowOff>242455</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="矢印: 右 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F462A3B-7B60-42B8-AD49-069454990E1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10633364" y="77031273"/>
+          <a:ext cx="1974272" cy="1524000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="stealth" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>69272</xdr:colOff>
+      <xdr:row>246</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>536864</xdr:colOff>
+      <xdr:row>248</xdr:row>
+      <xdr:rowOff>17318</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="正方形/長方形 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F515689-19AA-4136-9331-132F36DCDFB0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3463636" y="80945182"/>
+          <a:ext cx="4312228" cy="675409"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="stealth" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>536864</xdr:colOff>
+      <xdr:row>257</xdr:row>
+      <xdr:rowOff>138545</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>389262</xdr:colOff>
+      <xdr:row>268</xdr:row>
+      <xdr:rowOff>85712</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="図 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD874B86-23E8-4B69-9888-335B2E17EB6B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2008909" y="84703227"/>
+          <a:ext cx="10100000" cy="3561905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>103909</xdr:colOff>
+      <xdr:row>257</xdr:row>
+      <xdr:rowOff>212581</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>541392</xdr:colOff>
+      <xdr:row>265</xdr:row>
+      <xdr:rowOff>160627</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="図 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FB92A50-DF2B-469E-A242-E86DC0EC5494}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12469091" y="84777263"/>
+          <a:ext cx="8767528" cy="2580409"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>277091</xdr:colOff>
+      <xdr:row>274</xdr:row>
+      <xdr:rowOff>86591</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>170262</xdr:colOff>
+      <xdr:row>296</xdr:row>
+      <xdr:rowOff>123781</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="図 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{184300D9-D47C-4C00-8110-7BFF2D229DC1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2389909" y="90245046"/>
+          <a:ext cx="9504762" cy="7276190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>86591</xdr:colOff>
+      <xdr:row>291</xdr:row>
+      <xdr:rowOff>311728</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>277091</xdr:colOff>
+      <xdr:row>295</xdr:row>
+      <xdr:rowOff>138546</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="フローチャート: 処理 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7954F00B-9E8E-4D51-87B0-3D8E8C3A938B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2840182" y="96063955"/>
+          <a:ext cx="7879773" cy="1143000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartProcess">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="stealth" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>638819</xdr:colOff>
+      <xdr:row>277</xdr:row>
+      <xdr:rowOff>143307</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>606137</xdr:colOff>
+      <xdr:row>293</xdr:row>
+      <xdr:rowOff>17318</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="フリーフォーム: 図形 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B607845-5ED7-4252-9795-B1347B322167}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2751637" y="91288898"/>
+          <a:ext cx="6375045" cy="5138738"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 6206625 w 6206625"/>
+            <a:gd name="connsiteY0" fmla="*/ 5143500 h 5143500"/>
+            <a:gd name="connsiteX1" fmla="*/ 266489 w 6206625"/>
+            <a:gd name="connsiteY1" fmla="*/ 2528455 h 5143500"/>
+            <a:gd name="connsiteX2" fmla="*/ 1582670 w 6206625"/>
+            <a:gd name="connsiteY2" fmla="*/ 0 h 5143500"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="6206625" h="5143500">
+              <a:moveTo>
+                <a:pt x="6206625" y="5143500"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="3621886" y="4264602"/>
+                <a:pt x="1037148" y="3385705"/>
+                <a:pt x="266489" y="2528455"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="-504170" y="1671205"/>
+                <a:pt x="539250" y="835602"/>
+                <a:pt x="1582670" y="0"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="stealth" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>329045</xdr:colOff>
+      <xdr:row>293</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>207818</xdr:colOff>
+      <xdr:row>294</xdr:row>
+      <xdr:rowOff>103909</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="正方形/長方形 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0A84E86-40C6-42C3-985D-BD50EC0C335B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8208818" y="96410318"/>
+          <a:ext cx="1801091" cy="432955"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="stealth" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>311727</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>138546</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>225136</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>225137</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="テキスト ボックス 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0865FE4F-5B50-45C7-9FF7-58EEBBB22BFD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5628409" y="51140591"/>
+          <a:ext cx="8884227" cy="744682"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B0F0"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400"/>
+            <a:t>phần</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" baseline="0"/>
+            <a:t> này nhúng thêm ra ReactDOM vào.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="2400"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2055,19 +2733,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2983FCD5-2F3F-4DE5-AD03-9AA1FE5631D5}">
-  <dimension ref="A1:L207"/>
+  <dimension ref="A1:L273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C209" sqref="C209"/>
+    <sheetView tabSelected="1" topLeftCell="A187" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="X219" sqref="X219"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.0625" defaultRowHeight="32.25" x14ac:dyDescent="1.25"/>
+  <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="25.5"/>
   <cols>
-    <col min="1" max="1" width="20.4375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.0625" style="1"/>
+    <col min="1" max="1" width="20.46484375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="1.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2083,12 +2761,12 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="1.25">
+    <row r="2" spans="1:12">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="1.25">
+    <row r="28" spans="1:12">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -2104,17 +2782,17 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="1.25">
+    <row r="29" spans="1:12">
       <c r="B29" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="1.25">
+    <row r="31" spans="1:12">
       <c r="D31" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="1.25">
+    <row r="49" spans="1:12">
       <c r="A49" s="2" t="s">
         <v>5</v>
       </c>
@@ -2130,7 +2808,7 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="1.25">
+    <row r="144" spans="1:12">
       <c r="A144" s="2" t="s">
         <v>6</v>
       </c>
@@ -2146,12 +2824,12 @@
       <c r="K144" s="2"/>
       <c r="L144" s="2"/>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="1.25">
+    <row r="145" spans="2:2">
       <c r="B145" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="1.25">
+    <row r="178" spans="1:12">
       <c r="A178" s="2" t="s">
         <v>8</v>
       </c>
@@ -2167,7 +2845,7 @@
       <c r="K178" s="2"/>
       <c r="L178" s="2"/>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="1.25">
+    <row r="195" spans="1:12">
       <c r="A195" s="2" t="s">
         <v>9</v>
       </c>
@@ -2183,10 +2861,58 @@
       <c r="K195" s="2"/>
       <c r="L195" s="2"/>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="1.25">
+    <row r="207" spans="1:12">
       <c r="E207" s="1" t="s">
         <v>10</v>
       </c>
+    </row>
+    <row r="229" spans="1:12">
+      <c r="A229" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B229" s="2"/>
+      <c r="C229" s="2"/>
+      <c r="D229" s="2"/>
+      <c r="E229" s="2"/>
+      <c r="F229" s="2"/>
+      <c r="G229" s="2"/>
+      <c r="H229" s="2"/>
+      <c r="I229" s="2"/>
+      <c r="J229" s="2"/>
+      <c r="K229" s="2"/>
+      <c r="L229" s="2"/>
+    </row>
+    <row r="255" spans="1:12">
+      <c r="A255" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B255" s="2"/>
+      <c r="C255" s="2"/>
+      <c r="D255" s="2"/>
+      <c r="E255" s="2"/>
+      <c r="F255" s="2"/>
+      <c r="G255" s="2"/>
+      <c r="H255" s="2"/>
+      <c r="I255" s="2"/>
+      <c r="J255" s="2"/>
+      <c r="K255" s="2"/>
+      <c r="L255" s="2"/>
+    </row>
+    <row r="273" spans="1:12">
+      <c r="A273" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B273" s="2"/>
+      <c r="C273" s="2"/>
+      <c r="D273" s="2"/>
+      <c r="E273" s="2"/>
+      <c r="F273" s="2"/>
+      <c r="G273" s="2"/>
+      <c r="H273" s="2"/>
+      <c r="I273" s="2"/>
+      <c r="J273" s="2"/>
+      <c r="K273" s="2"/>
+      <c r="L273" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3"/>
@@ -2204,7 +2930,7 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update to latest react and react dom
</commit_message>
<xml_diff>
--- a/ReactjswithF8.xlsx
+++ b/ReactjswithF8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cng\0_personal\2_Reactjs\1_Reactjs_with_F8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A03F25-3F70-46A2-8238-B66988A9AAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E39F04B-E9EA-4997-A789-482314CE9CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57165" yWindow="1530" windowWidth="21600" windowHeight="11430" activeTab="3" xr2:uid="{4149283A-B59B-4AE5-95CD-24380AF48A33}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>Rest trong js là gì?</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>npm install webpack-dev-server --save-dev</t>
+  </si>
+  <si>
+    <t>npm i react@latest react-dom@latest</t>
   </si>
 </sst>
 </file>
@@ -7813,10 +7816,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45273496-BEF3-4F89-B9B1-72849BD4328E}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="X15" sqref="X15"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5"/>
@@ -7911,6 +7914,11 @@
         <v>47</v>
       </c>
     </row>
+    <row r="29" spans="1:12">
+      <c r="B29" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J19" r:id="rId1" xr:uid="{20384AD6-2941-4241-BE3C-C3AF5E3A631C}"/>

</xml_diff>

<commit_message>
create reactAPP - very fast
</commit_message>
<xml_diff>
--- a/ReactjswithF8.xlsx
+++ b/ReactjswithF8.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cng\0_personal\2_Reactjs\1_Reactjs_with_F8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E39F04B-E9EA-4997-A789-482314CE9CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90613F89-7566-4A64-B878-1258B2276ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57165" yWindow="1530" windowWidth="21600" windowHeight="11430" activeTab="3" xr2:uid="{4149283A-B59B-4AE5-95CD-24380AF48A33}"/>
+    <workbookView xWindow="64005" yWindow="2595" windowWidth="21600" windowHeight="11430" activeTab="3" xr2:uid="{4149283A-B59B-4AE5-95CD-24380AF48A33}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>Rest trong js là gì?</t>
   </si>
@@ -180,6 +180,12 @@
   </si>
   <si>
     <t>npm i react@latest react-dom@latest</t>
+  </si>
+  <si>
+    <t>npx create-react-app tiktok</t>
+  </si>
+  <si>
+    <t>3.Create ReactAPP_create tiktok react project sieu nhanh voi cmd cua facebook</t>
   </si>
 </sst>
 </file>
@@ -7816,10 +7822,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45273496-BEF3-4F89-B9B1-72849BD4328E}">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5"/>
@@ -7919,6 +7925,27 @@
         <v>48</v>
       </c>
     </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="B36" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J19" r:id="rId1" xr:uid="{20384AD6-2941-4241-BE3C-C3AF5E3A631C}"/>

</xml_diff>